<commit_message>
file updates, var1a working
</commit_message>
<xml_diff>
--- a/Data/totalCSWP.xlsx
+++ b/Data/totalCSWP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="0" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
+    <workbookView xWindow="8000" yWindow="860" windowWidth="25600" windowHeight="14540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -320,7 +320,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -328,767 +328,1220 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A151"/>
+  <dimension ref="A1:B151"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection sqref="A1:A151"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1">
         <v>389656843.19585478</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1">
+        <v>388732049.37306201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>437223238.72604603</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2">
+        <v>435517399.74874842</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>485815953.94297212</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="B3">
+        <v>483534639.8012408</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>535634773.92423928</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="B4">
+        <v>532374177.01852596</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>586323753.03475094</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="B5">
+        <v>582030678.38475871</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>637147075.62747848</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="B6">
+        <v>632104240.70372951</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>691452875.15862989</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="B7">
+        <v>685584327.63132763</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>748996033.5582974</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="B8">
+        <v>742093869.87204933</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>799751991.57193506</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="B9">
+        <v>792096107.14280581</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>853415692.07252181</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="B10">
+        <v>845059292.00092244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>906491919.83012581</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
+      <c r="B11">
+        <v>897127505.24545813</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>956615441.27641511</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
+      <c r="B12">
+        <v>945825504.25309944</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13">
         <v>1007491363.0212278</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
+      <c r="B13">
+        <v>995183975.86333227</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14">
         <v>1056357941.4937975</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
+      <c r="B14">
+        <v>1042411131.8684185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15">
         <v>1100437295.5076444</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
+      <c r="B15">
+        <v>1085646721.4077406</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16">
         <v>1139971857.9019358</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16">
+        <v>1125105046.5786452</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>1181979729.3363106</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17">
+        <v>1167198501.300457</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18">
         <v>1219510919.5704572</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18">
+        <v>1204875770.1426172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19">
         <v>1253160421.9499819</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19">
+        <v>1238713921.9022229</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20">
         <v>1288627890.091064</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20">
+        <v>1273927168.0064287</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21">
         <v>1323564806.9639084</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21">
+        <v>1308669555.5747819</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22">
         <v>1350343998.8898625</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="B22">
+        <v>1335195559.8843431</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23">
         <v>1381418710.5846422</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="B23">
+        <v>1366042418.0291548</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24">
         <v>1417143003.1317844</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="B24">
+        <v>1401446158.8848109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25">
         <v>1450595037.0048509</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
+      <c r="B25">
+        <v>1434164701.4525414</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26">
         <v>1482453121.647876</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
+      <c r="B26">
+        <v>1465491638.3349884</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27">
         <v>1512832806.6109838</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="B27">
+        <v>1495229480.1888566</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28">
         <v>1540024013.3976495</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="B28">
+        <v>1521458732.324043</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29">
         <v>1565588909.9124417</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="B29">
+        <v>1545691424.4271708</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30">
         <v>1592791071.9514647</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="B30">
+        <v>1571675896.33779</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31">
         <v>1609106006.6319568</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="B31">
+        <v>1587201083.785594</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32">
         <v>1614126694.6971664</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="B32">
+        <v>1591634496.4312615</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33">
         <v>1611702856.9412575</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="B33">
+        <v>1588819591.3690777</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34">
         <v>1612438748.3344707</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
+      <c r="B34">
+        <v>1589032118.4082298</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35">
         <v>1615109724.0843306</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="B35">
+        <v>1591078163.211771</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36">
         <v>1621669227.3154974</v>
       </c>
-    </row>
-    <row r="37" spans="1:1">
+      <c r="B36">
+        <v>1597142161.6147118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37">
         <v>1633233879.7525551</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
+      <c r="B37">
+        <v>1608399539.2841647</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38">
         <v>1646435001.1792781</v>
       </c>
-    </row>
-    <row r="39" spans="1:1">
+      <c r="B38">
+        <v>1621173009.2655077</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
       <c r="A39">
         <v>1654525776.4670565</v>
       </c>
-    </row>
-    <row r="40" spans="1:1">
+      <c r="B39">
+        <v>1629162389.1512589</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40">
         <v>1666506225.7275274</v>
       </c>
-    </row>
-    <row r="41" spans="1:1">
+      <c r="B40">
+        <v>1641092218.1716621</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
       <c r="A41">
         <v>1680279603.4842005</v>
       </c>
-    </row>
-    <row r="42" spans="1:1">
+      <c r="B41">
+        <v>1654928619.4533789</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
       <c r="A42">
         <v>1699869288.059917</v>
       </c>
-    </row>
-    <row r="43" spans="1:1">
+      <c r="B42">
+        <v>1675258053.6519547</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
       <c r="A43">
         <v>1718999923.6333818</v>
       </c>
-    </row>
-    <row r="44" spans="1:1">
+      <c r="B43">
+        <v>1695382662.2875171</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
       <c r="A44">
         <v>1735314952.5593953</v>
       </c>
-    </row>
-    <row r="45" spans="1:1">
+      <c r="B44">
+        <v>1712156596.4730978</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
       <c r="A45">
         <v>1750325153.3065078</v>
       </c>
-    </row>
-    <row r="46" spans="1:1">
+      <c r="B45">
+        <v>1727780882.535521</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
       <c r="A46">
         <v>1760205914.3968132</v>
       </c>
-    </row>
-    <row r="47" spans="1:1">
+      <c r="B46">
+        <v>1738347628.8771529</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
       <c r="A47">
         <v>1775662444.5789378</v>
       </c>
-    </row>
-    <row r="48" spans="1:1">
+      <c r="B47">
+        <v>1754479756.0557332</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
       <c r="A48">
         <v>1792474326.126893</v>
       </c>
-    </row>
-    <row r="49" spans="1:1">
+      <c r="B48">
+        <v>1771386465.6370535</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49">
         <v>1809173298.4365511</v>
       </c>
-    </row>
-    <row r="50" spans="1:1">
+      <c r="B49">
+        <v>1789313091.5588658</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
       <c r="A50">
         <v>1819492168.0190277</v>
       </c>
-    </row>
-    <row r="51" spans="1:1">
+      <c r="B50">
+        <v>1800570787.7477524</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
       <c r="A51">
         <v>1835029595.0470643</v>
       </c>
-    </row>
-    <row r="52" spans="1:1">
+      <c r="B51">
+        <v>1818871464.6137338</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
       <c r="A52">
         <v>1847623592.7745445</v>
       </c>
-    </row>
-    <row r="53" spans="1:1">
+      <c r="B52">
+        <v>1833139774.1822357</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
       <c r="A53">
         <v>1859739145.9743848</v>
       </c>
-    </row>
-    <row r="54" spans="1:1">
+      <c r="B53">
+        <v>1846854798.6588831</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
       <c r="A54">
         <v>1871360581.6414549</v>
       </c>
-    </row>
-    <row r="55" spans="1:1">
+      <c r="B54">
+        <v>1860447188.8666005</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
       <c r="A55">
         <v>1882349761.9673543</v>
       </c>
-    </row>
-    <row r="56" spans="1:1">
+      <c r="B55">
+        <v>1873679775.5020483</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
       <c r="A56">
         <v>1894761766.7395563</v>
       </c>
-    </row>
-    <row r="57" spans="1:1">
+      <c r="B56">
+        <v>1888553013.9299889</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
       <c r="A57">
         <v>1907595878.6065559</v>
       </c>
-    </row>
-    <row r="58" spans="1:1">
+      <c r="B57">
+        <v>1903747350.7787859</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
       <c r="A58">
         <v>1915011592.0775523</v>
       </c>
-    </row>
-    <row r="59" spans="1:1">
+      <c r="B58">
+        <v>1913075329.3518505</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
       <c r="A59">
         <v>1923104451.2515507</v>
       </c>
-    </row>
-    <row r="60" spans="1:1">
+      <c r="B59">
+        <v>1923424778.0743873</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
       <c r="A60">
         <v>1934798390.6792412</v>
       </c>
-    </row>
-    <row r="61" spans="1:1">
+      <c r="B60">
+        <v>1937991524.8550913</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
       <c r="A61">
         <v>1942504009.904635</v>
       </c>
-    </row>
-    <row r="62" spans="1:1">
+      <c r="B61">
+        <v>1948188912.2760987</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
       <c r="A62">
         <v>1949817585.3592472</v>
       </c>
-    </row>
-    <row r="63" spans="1:1">
+      <c r="B62">
+        <v>1957986751.6647735</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
       <c r="A63">
         <v>1958417521.6428785</v>
       </c>
-    </row>
-    <row r="64" spans="1:1">
+      <c r="B63">
+        <v>1969760419.9824638</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
       <c r="A64">
         <v>1970302941.1726561</v>
       </c>
-    </row>
-    <row r="65" spans="1:1">
+      <c r="B64">
+        <v>1984637566.5060356</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
       <c r="A65">
         <v>1984776231.593184</v>
       </c>
-    </row>
-    <row r="66" spans="1:1">
+      <c r="B65">
+        <v>2001804356.0012527</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
       <c r="A66">
         <v>2002330065.4513638</v>
       </c>
-    </row>
-    <row r="67" spans="1:1">
+      <c r="B66">
+        <v>2022063587.0952096</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
       <c r="A67">
         <v>2020358747.4500315</v>
       </c>
-    </row>
-    <row r="68" spans="1:1">
+      <c r="B67">
+        <v>2042473058.7398171</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
       <c r="A68">
         <v>2037009049.3629086</v>
       </c>
-    </row>
-    <row r="69" spans="1:1">
+      <c r="B68">
+        <v>2060743597.7848616</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
       <c r="A69">
         <v>2055467575.9731295</v>
       </c>
-    </row>
-    <row r="70" spans="1:1">
+      <c r="B69">
+        <v>2081491501.784734</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
       <c r="A70">
         <v>2073967142.3924487</v>
       </c>
-    </row>
-    <row r="71" spans="1:1">
+      <c r="B70">
+        <v>2102594227.0514801</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
       <c r="A71">
         <v>2092043818.3584888</v>
       </c>
-    </row>
-    <row r="72" spans="1:1">
+      <c r="B71">
+        <v>2122853012.7464199</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
       <c r="A72">
         <v>2113169051.5297117</v>
       </c>
-    </row>
-    <row r="73" spans="1:1">
+      <c r="B72">
+        <v>2147675903.9649777</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
       <c r="A73">
         <v>2136141832.7466304</v>
       </c>
-    </row>
-    <row r="74" spans="1:1">
+      <c r="B73">
+        <v>2174928423.7334852</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
       <c r="A74">
         <v>2159881024.4835129</v>
       </c>
-    </row>
-    <row r="75" spans="1:1">
+      <c r="B74">
+        <v>2201899976.76579</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
       <c r="A75">
         <v>2176368934.0413551</v>
       </c>
-    </row>
-    <row r="76" spans="1:1">
+      <c r="B75">
+        <v>2220103285.778368</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
       <c r="A76">
         <v>2189142648.2544675</v>
       </c>
-    </row>
-    <row r="77" spans="1:1">
+      <c r="B76">
+        <v>2233672654.1657801</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
       <c r="A77">
         <v>2207530466.9861155</v>
       </c>
-    </row>
-    <row r="78" spans="1:1">
+      <c r="B77">
+        <v>2254013329.3702869</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
       <c r="A78">
         <v>2228948878.0906224</v>
       </c>
-    </row>
-    <row r="79" spans="1:1">
+      <c r="B78">
+        <v>2279912134.7328777</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
       <c r="A79">
         <v>2251850142.0838919</v>
       </c>
-    </row>
-    <row r="80" spans="1:1">
+      <c r="B79">
+        <v>2307994564.9913836</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
       <c r="A80">
         <v>2274348137.5880699</v>
       </c>
-    </row>
-    <row r="81" spans="1:1">
+      <c r="B80">
+        <v>2334070576.5797315</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
       <c r="A81">
         <v>2289667985.6178951</v>
       </c>
-    </row>
-    <row r="82" spans="1:1">
+      <c r="B81">
+        <v>2351578900.6798277</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
       <c r="A82">
         <v>2300960774.4692373</v>
       </c>
-    </row>
-    <row r="83" spans="1:1">
+      <c r="B82">
+        <v>2365497961.2306876</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
       <c r="A83">
         <v>2311957218.6760106</v>
       </c>
-    </row>
-    <row r="84" spans="1:1">
+      <c r="B83">
+        <v>2379552863.6506243</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
       <c r="A84">
         <v>2331904123.0040159</v>
       </c>
-    </row>
-    <row r="85" spans="1:1">
+      <c r="B84">
+        <v>2404831569.777607</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
       <c r="A85">
         <v>2355133348.820817</v>
       </c>
-    </row>
-    <row r="86" spans="1:1">
+      <c r="B85">
+        <v>2434928670.1385074</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
       <c r="A86">
         <v>2378443226.4848413</v>
       </c>
-    </row>
-    <row r="87" spans="1:1">
+      <c r="B86">
+        <v>2466134878.1186919</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
       <c r="A87">
         <v>2406795969.2063608</v>
       </c>
-    </row>
-    <row r="88" spans="1:1">
+      <c r="B87">
+        <v>2501564349.7383966</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
       <c r="A88">
         <v>2439433712.8990016</v>
       </c>
-    </row>
-    <row r="89" spans="1:1">
+      <c r="B88">
+        <v>2540902842.4975615</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
       <c r="A89">
         <v>2473277026.2187462</v>
       </c>
-    </row>
-    <row r="90" spans="1:1">
+      <c r="B89">
+        <v>2577869016.2915802</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
       <c r="A90">
         <v>2507032595.7482305</v>
       </c>
-    </row>
-    <row r="91" spans="1:1">
+      <c r="B90">
+        <v>2613964842.0034332</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
       <c r="A91">
         <v>2538693596.6428919</v>
       </c>
-    </row>
-    <row r="92" spans="1:1">
+      <c r="B91">
+        <v>2646761362.9246211</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
       <c r="A92">
         <v>2564882702.4099097</v>
       </c>
-    </row>
-    <row r="93" spans="1:1">
+      <c r="B92">
+        <v>2673035704.7653322</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
       <c r="A93">
         <v>2592740383.1683764</v>
       </c>
-    </row>
-    <row r="94" spans="1:1">
+      <c r="B93">
+        <v>2703355843.6116123</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
       <c r="A94">
         <v>2619668467.918571</v>
       </c>
-    </row>
-    <row r="95" spans="1:1">
+      <c r="B94">
+        <v>2735338384.078022</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
       <c r="A95">
         <v>2646393294.2087274</v>
       </c>
-    </row>
-    <row r="96" spans="1:1">
+      <c r="B95">
+        <v>2768769958.7850785</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
       <c r="A96">
         <v>2671160602.8903418</v>
       </c>
-    </row>
-    <row r="97" spans="1:1">
+      <c r="B96">
+        <v>2801338950.6212215</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
       <c r="A97">
         <v>2696430161.2166786</v>
       </c>
-    </row>
-    <row r="98" spans="1:1">
+      <c r="B97">
+        <v>2835741846.5561924</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
       <c r="A98">
         <v>2722349173.0367541</v>
       </c>
-    </row>
-    <row r="99" spans="1:1">
+      <c r="B98">
+        <v>2871557867.4132466</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
       <c r="A99">
         <v>2747440883.7917299</v>
       </c>
-    </row>
-    <row r="100" spans="1:1">
+      <c r="B99">
+        <v>2909461717.2506099</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
       <c r="A100">
         <v>2774210114.167881</v>
       </c>
-    </row>
-    <row r="101" spans="1:1">
+      <c r="B100">
+        <v>2949936690.7443137</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
       <c r="A101">
         <v>2800357395.2847004</v>
       </c>
-    </row>
-    <row r="102" spans="1:1">
+      <c r="B101">
+        <v>2989985216.8559184</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
       <c r="A102">
         <v>2822573761.8943901</v>
       </c>
-    </row>
-    <row r="103" spans="1:1">
+      <c r="B102">
+        <v>3027433541.1109128</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
       <c r="A103">
         <v>2846096428.5869803</v>
       </c>
-    </row>
-    <row r="104" spans="1:1">
+      <c r="B103">
+        <v>3067032561.6436782</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
       <c r="A104">
         <v>2867921752.3019114</v>
       </c>
-    </row>
-    <row r="105" spans="1:1">
+      <c r="B104">
+        <v>3105954761.2912154</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
       <c r="A105">
         <v>2892776889.2836533</v>
       </c>
-    </row>
-    <row r="106" spans="1:1">
+      <c r="B105">
+        <v>3151841936.6596775</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
       <c r="A106">
         <v>2917679759.8848152</v>
       </c>
-    </row>
-    <row r="107" spans="1:1">
+      <c r="B106">
+        <v>3198510092.4643612</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
       <c r="A107">
         <v>2940765110.2871881</v>
       </c>
-    </row>
-    <row r="108" spans="1:1">
+      <c r="B107">
+        <v>3240154427.1422944</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
       <c r="A108">
         <v>2959512311.6914454</v>
       </c>
-    </row>
-    <row r="109" spans="1:1">
+      <c r="B108">
+        <v>3270837460.0894337</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
       <c r="A109">
         <v>2965821012.111145</v>
       </c>
-    </row>
-    <row r="110" spans="1:1">
+      <c r="B109">
+        <v>3281687638.6861758</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
       <c r="A110">
         <v>2964690550.1407099</v>
       </c>
-    </row>
-    <row r="111" spans="1:1">
+      <c r="B110">
+        <v>3281768476.0473647</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
       <c r="A111">
         <v>2964308017.547183</v>
       </c>
-    </row>
-    <row r="112" spans="1:1">
+      <c r="B111">
+        <v>3282069463.3337517</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
       <c r="A112">
         <v>2966945773.6524258</v>
       </c>
-    </row>
-    <row r="113" spans="1:1">
+      <c r="B112">
+        <v>3284479932.0473142</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
       <c r="A113">
         <v>2970683079.1117067</v>
       </c>
-    </row>
-    <row r="114" spans="1:1">
+      <c r="B113">
+        <v>3289334069.6384697</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
       <c r="A114">
         <v>2977443518.8774414</v>
       </c>
-    </row>
-    <row r="115" spans="1:1">
+      <c r="B114">
+        <v>3298536683.2935319</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
       <c r="A115">
         <v>2985851215.9569564</v>
       </c>
-    </row>
-    <row r="116" spans="1:1">
+      <c r="B115">
+        <v>3312091178.2823668</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
       <c r="A116">
         <v>2996456638.3327913</v>
       </c>
-    </row>
-    <row r="117" spans="1:1">
+      <c r="B116">
+        <v>3329495393.2350278</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
       <c r="A117">
         <v>3009221478.5042706</v>
       </c>
-    </row>
-    <row r="118" spans="1:1">
+      <c r="B117">
+        <v>3350685164.1238737</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
       <c r="A118">
         <v>3024108271.5067968</v>
       </c>
-    </row>
-    <row r="119" spans="1:1">
+      <c r="B118">
+        <v>3375597591.4649363</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
       <c r="A119">
         <v>3041080365.0354729</v>
       </c>
-    </row>
-    <row r="120" spans="1:1">
+      <c r="B119">
+        <v>3404171012.704771</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
       <c r="A120">
         <v>3060101892.20298</v>
       </c>
-    </row>
-    <row r="121" spans="1:1">
+      <c r="B120">
+        <v>3436344975.253243</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
       <c r="A121">
         <v>3080862962.1888032</v>
       </c>
-    </row>
-    <row r="122" spans="1:1">
+      <c r="B121">
+        <v>3475072097.2092156</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
       <c r="A122">
         <v>3109265319.7730393</v>
       </c>
-    </row>
-    <row r="123" spans="1:1">
+      <c r="B122">
+        <v>3517725189.12988</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
       <c r="A123">
         <v>3137711385.2582684</v>
       </c>
-    </row>
-    <row r="124" spans="1:1">
+      <c r="B123">
+        <v>3560228835.4704089</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
       <c r="A124">
         <v>3166348249.1337576</v>
       </c>
-    </row>
-    <row r="125" spans="1:1">
+      <c r="B124">
+        <v>3602802615.5553164</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
       <c r="A125">
         <v>3195077805.0832367</v>
       </c>
-    </row>
-    <row r="126" spans="1:1">
+      <c r="B125">
+        <v>3645381654.4502387</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
       <c r="A126">
         <v>3223592823.0698137</v>
       </c>
-    </row>
-    <row r="127" spans="1:1">
+      <c r="B126">
+        <v>3687521361.3436856</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
       <c r="A127">
         <v>3251732534.9123645</v>
       </c>
-    </row>
-    <row r="128" spans="1:1">
+      <c r="B127">
+        <v>3729144324.0885363</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
       <c r="A128">
         <v>3279685709.2633152</v>
       </c>
-    </row>
-    <row r="129" spans="1:1">
+      <c r="B128">
+        <v>3770702546.635406</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
       <c r="A129">
         <v>3307405040.9677124</v>
       </c>
-    </row>
-    <row r="130" spans="1:1">
+      <c r="B129">
+        <v>3811976913.086112</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
       <c r="A130">
         <v>3335028954.7768664</v>
       </c>
-    </row>
-    <row r="131" spans="1:1">
+      <c r="B130">
+        <v>3853043571.5148287</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
       <c r="A131">
         <v>3362562630.7032099</v>
       </c>
-    </row>
-    <row r="132" spans="1:1">
+      <c r="B131">
+        <v>3893877660.5743957</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
       <c r="A132">
         <v>3390437565.1407242</v>
       </c>
-    </row>
-    <row r="133" spans="1:1">
+      <c r="B132">
+        <v>3935227896.1654549</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
       <c r="A133">
         <v>3418257821.1067739</v>
       </c>
-    </row>
-    <row r="134" spans="1:1">
+      <c r="B133">
+        <v>3976296365.2456479</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
       <c r="A134">
         <v>3446082442.9488559</v>
       </c>
-    </row>
-    <row r="135" spans="1:1">
+      <c r="B134">
+        <v>4017599097.9148932</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
       <c r="A135">
         <v>3474032478.0715108</v>
       </c>
-    </row>
-    <row r="136" spans="1:1">
+      <c r="B135">
+        <v>4059175411.6554146</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
       <c r="A136">
         <v>3501928117.9174714</v>
       </c>
-    </row>
-    <row r="137" spans="1:1">
+      <c r="B136">
+        <v>4100757014.2615557</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
       <c r="A137">
         <v>3530042534.5184145</v>
       </c>
-    </row>
-    <row r="138" spans="1:1">
+      <c r="B137">
+        <v>4142646216.8030672</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
       <c r="A138">
         <v>3558233763.8585868</v>
       </c>
-    </row>
-    <row r="139" spans="1:1">
+      <c r="B138">
+        <v>4184547243.268188</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
       <c r="A139">
         <v>3586497650.5681043</v>
       </c>
-    </row>
-    <row r="140" spans="1:1">
+      <c r="B139">
+        <v>4226309201.8148375</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
       <c r="A140">
         <v>3614949742.378037</v>
       </c>
-    </row>
-    <row r="141" spans="1:1">
+      <c r="B140">
+        <v>4268160754.5260568</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
       <c r="A141">
         <v>3643706437.4867463</v>
       </c>
-    </row>
-    <row r="142" spans="1:1">
+      <c r="B141">
+        <v>4310328279.1518965</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
       <c r="A142">
         <v>3672821547.5649023</v>
       </c>
-    </row>
-    <row r="143" spans="1:1">
+      <c r="B142">
+        <v>4352866692.6805372</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
       <c r="A143">
         <v>3702192497.3414698</v>
       </c>
-    </row>
-    <row r="144" spans="1:1">
+      <c r="B143">
+        <v>4396000218.5721416</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
       <c r="A144">
         <v>3731875758.616118</v>
       </c>
-    </row>
-    <row r="145" spans="1:1">
+      <c r="B144">
+        <v>4439693189.0058565</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
       <c r="A145">
         <v>3761767705.4655275</v>
       </c>
-    </row>
-    <row r="146" spans="1:1">
+      <c r="B145">
+        <v>4483553480.1147957</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
       <c r="A146">
         <v>3791890649.3883138</v>
       </c>
-    </row>
-    <row r="147" spans="1:1">
+      <c r="B146">
+        <v>4527836473.8331614</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
       <c r="A147">
         <v>3822152380.5814319</v>
       </c>
-    </row>
-    <row r="148" spans="1:1">
+      <c r="B147">
+        <v>4572265451.2191219</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
       <c r="A148">
         <v>3852674771.0872951</v>
       </c>
-    </row>
-    <row r="149" spans="1:1">
+      <c r="B148">
+        <v>4616888599.4075251</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
       <c r="A149">
         <v>3883393304.2495294</v>
       </c>
-    </row>
-    <row r="150" spans="1:1">
+      <c r="B149">
+        <v>4661732241.6107826</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
       <c r="A150">
         <v>3914401859.1251478</v>
       </c>
-    </row>
-    <row r="151" spans="1:1">
+      <c r="B150">
+        <v>4706766431.7790003</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
       <c r="A151">
         <v>3945606868.6721969</v>
+      </c>
+      <c r="B151">
+        <v>4751949775.4672346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>